<commit_message>
change mapping.py path, add choses.py
</commit_message>
<xml_diff>
--- a/output/planilhas/leilaoimoveis_caninde-ce.xlsx
+++ b/output/planilhas/leilaoimoveis_caninde-ce.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -749,6 +749,150 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Outros </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>05/03/2024</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Judicial</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Norte Nordeste Leilões </t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>R. RAIMUNDO ALCONFORADO, Nº 158</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/caninde/outros-predio-2-andares-terreno-200m-caninde-ce-desocupado-imovel-1627069</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Outros </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>05/03/2024</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Judicial</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Norte Nordeste Leilões </t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>RUA JOSÉ VELOSO JUCÁ, N° 2576</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/caninde/outros-predio-triplex-terreno-130m-caninde-ce-imovel-1627070</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Outros </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>05/03/2024</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Judicial</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Norte Nordeste Leilões </t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>TRAVESSA JOÃO MARTINS, N° 56</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/caninde/outros-predio-2-pavs-196-20m-terreno-150m-caninde-ce-imovel-1627068</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>